<commit_message>
transition rule 5 and 10 mi rad updates to script and all outputs
</commit_message>
<xml_diff>
--- a/output/Transitions Rule/facility_data/transition_rule_facility_demographics_1mi.xlsx
+++ b/output/Transitions Rule/facility_data/transition_rule_facility_demographics_1mi.xlsx
@@ -594,10 +594,10 @@
         <v>6.35288902024531</v>
       </c>
       <c r="R2" t="n">
-        <v>40.0487722284549</v>
+        <v>35</v>
       </c>
       <c r="S2" t="n">
-        <v>0.55881633905</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="3">
@@ -653,10 +653,10 @@
         <v>6.92743033168565</v>
       </c>
       <c r="R3" t="n">
-        <v>53.5633054085323</v>
+        <v>50</v>
       </c>
       <c r="S3" t="n">
-        <v>0.677420520359875</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4">
@@ -710,10 +710,10 @@
         <v>3.49961154043405</v>
       </c>
       <c r="R4" t="n">
-        <v>38.3988393274612</v>
+        <v>40</v>
       </c>
       <c r="S4" t="n">
-        <v>0.580259286776863</v>
+        <v>0.442857142857143</v>
       </c>
     </row>
     <row r="5">
@@ -767,10 +767,10 @@
         <v>12.93324635522</v>
       </c>
       <c r="R5" t="n">
-        <v>35.6968955479137</v>
+        <v>30</v>
       </c>
       <c r="S5" t="n">
-        <v>0.612398370663204</v>
+        <v>0.485714285714286</v>
       </c>
     </row>
     <row r="6">
@@ -824,10 +824,10 @@
         <v>0.595632031767042</v>
       </c>
       <c r="R6" t="n">
-        <v>25.9253212363581</v>
+        <v>30</v>
       </c>
       <c r="S6" t="n">
-        <v>0.345349221028167</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7">
@@ -883,10 +883,10 @@
         <v>12.0624622869681</v>
       </c>
       <c r="R7" t="n">
-        <v>30.6576927136365</v>
+        <v>30</v>
       </c>
       <c r="S7" t="n">
-        <v>0.393983274867232</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8">
@@ -942,10 +942,10 @@
         <v>3.03546019336931</v>
       </c>
       <c r="R8" t="n">
-        <v>18.5726437681445</v>
+        <v>20</v>
       </c>
       <c r="S8" t="n">
-        <v>0.23709346295086</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9">
@@ -1001,10 +1001,10 @@
         <v>2.76124521801586</v>
       </c>
       <c r="R9" t="n">
-        <v>109.314314527528</v>
+        <v>90</v>
       </c>
       <c r="S9" t="n">
-        <v>0.692666515625971</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10">
@@ -1060,10 +1060,10 @@
         <v>3.76813326109933</v>
       </c>
       <c r="R10" t="n">
-        <v>113.583851851753</v>
+        <v>107.5</v>
       </c>
       <c r="S10" t="n">
-        <v>0.752476122065753</v>
+        <v>0.525</v>
       </c>
     </row>
     <row r="11">
@@ -1117,10 +1117,10 @@
         <v>15.5423051839657</v>
       </c>
       <c r="R11" t="n">
-        <v>40.3605441928673</v>
+        <v>40</v>
       </c>
       <c r="S11" t="n">
-        <v>0.564902848349993</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12">
@@ -1174,10 +1174,10 @@
         <v>4.54580233864955</v>
       </c>
       <c r="R12" t="n">
-        <v>35.9317638652717</v>
+        <v>30</v>
       </c>
       <c r="S12" t="n">
-        <v>0.415944373765059</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="13">
@@ -1233,10 +1233,10 @@
         <v>10.1720400019476</v>
       </c>
       <c r="R13" t="n">
-        <v>65.3381786610065</v>
+        <v>40</v>
       </c>
       <c r="S13" t="n">
-        <v>0.85070990491521</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14">
@@ -1292,10 +1292,10 @@
         <v>1.0644418872267</v>
       </c>
       <c r="R14" t="n">
-        <v>17.8138934584248</v>
+        <v>20</v>
       </c>
       <c r="S14" t="n">
-        <v>0.213443064401811</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15">
@@ -1349,10 +1349,10 @@
         <v>10.2232142857143</v>
       </c>
       <c r="R15" t="n">
-        <v>32.4540319251191</v>
+        <v>30</v>
       </c>
       <c r="S15" t="n">
-        <v>0.465510184908126</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>